<commit_message>
updated code for new experiment execution
Comparison experiments changed. Project documents added
</commit_message>
<xml_diff>
--- a/Graphs/bf_ibf_03_06_2014.xlsx
+++ b/Graphs/bf_ibf_03_06_2014.xlsx
@@ -22,7 +22,7 @@
     <t>BloomFilter</t>
   </si>
   <si>
-    <t>ImpBloomFilter</t>
+    <t>ImpAwareBloomFilter</t>
   </si>
 </sst>
 </file>
@@ -574,12 +574,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>FalsePositive</a:t>
+              <a:t>False Positive Rate</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-IN" baseline="0"/>
-              <a:t> Vs TotalRequests</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-IN" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -694,7 +691,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ImpBloomFilter</c:v>
+                  <c:v>ImpAwareBloomFilter</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -781,14 +778,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="92108288"/>
-        <c:axId val="92109824"/>
+        <c:axId val="102802176"/>
+        <c:axId val="102804096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92108288"/>
+        <c:axId val="102802176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,14 +810,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92109824"/>
+        <c:crossAx val="102804096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92109824"/>
+        <c:axId val="102804096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -848,7 +844,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92108288"/>
+        <c:crossAx val="102802176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="200"/>
@@ -862,7 +858,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1191,7 +1187,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>